<commit_message>
There will bw big chandes
</commit_message>
<xml_diff>
--- a/surfaceTempDay.xlsx
+++ b/surfaceTempDay.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm\SC209\SC_209_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2428E718-FFA2-4335-8929-081B30AE8853}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0CFF62-1141-427A-A2A3-FB15706294CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suraceTempDay" sheetId="1" r:id="rId1"/>
@@ -1354,7 +1354,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2189,12 +2189,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B442"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A432" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2464,6 +2469,9 @@
       <c r="A34" t="s">
         <v>34</v>
       </c>
+      <c r="B34" s="1">
+        <v>15299</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">

</xml_diff>